<commit_message>
Update models 7/1/2025 11:46 AM UTC +6
</commit_message>
<xml_diff>
--- a/saved_models/accuracies/max_r_model_accuracies.xlsx
+++ b/saved_models/accuracies/max_r_model_accuracies.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9577922077922078</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7662337662337663</v>
+        <v>0.7694805194805194</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.961038961038961</v>
+        <v>0.9675324675324676</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7532467532467533</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         <v>0.9707792207792207</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7532467532467533</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.961038961038961</v>
+        <v>0.974025974025974</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7727272727272727</v>
+        <v>0.762987012987013</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9642857142857143</v>
+        <v>0.9675324675324676</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7402597402597403</v>
+        <v>0.7305194805194806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update saved model new model 3134 7/4/2025 5Trade
</commit_message>
<xml_diff>
--- a/saved_models/accuracies/max_r_model_accuracies.xlsx
+++ b/saved_models/accuracies/max_r_model_accuracies.xlsx
@@ -460,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5">
@@ -499,7 +499,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>